<commit_message>
motor control thermal start
</commit_message>
<xml_diff>
--- a/Power.xlsx
+++ b/Power.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\UdeS_S7_APP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25043BC0-A88F-4097-B141-4DE0332D274B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2447F5B4-6C78-46B9-8896-7EB82D8467DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50520" yWindow="5655" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Down Current</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Down Power</t>
   </si>
 </sst>
 </file>
@@ -147,12 +153,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -167,15 +209,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -450,60 +507,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -514,257 +572,604 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>24</v>
       </c>
-      <c r="D3">
-        <f>SUM(E3:Q3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="10">
+        <f t="shared" ref="C3:C16" si="0">D3 / B3</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10">
+        <f>F3 * B3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <f>SUM(G3:S3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="10">
         <v>12</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D17" si="0">SUM(E4:Q4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10">
+        <f>F4 * B4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" ref="F4:F17" si="1">SUM(G4:S4)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="10">
         <v>24</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
+      <c r="C5" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10">
+        <f>F5 * B5</f>
+        <v>48</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L5">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="O5" s="10"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="10">
         <v>5</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
+      <c r="C6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10">
+        <f>F6 * B6</f>
+        <v>0.19</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="1"/>
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="L6">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="10">
         <f>0.0212+0.0168</f>
         <v>3.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="O6" s="10"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>2.5</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <f>F7 * B7</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>1.5</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <f>F8 * B8</f>
+        <v>1.125</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="J8" s="5"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0.75</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <f>F9 * B9</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>3.3</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3005954545454532</v>
+      </c>
+      <c r="D10" s="1">
+        <f>E10 + (B10 - B11) * D11 + (B10 - B12) *D12</f>
+        <v>14.191964999999996</v>
+      </c>
+      <c r="E10" s="1">
+        <f>F10 * B10</f>
+        <v>5.0524649999999998</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
         <v>1.53105</v>
       </c>
-      <c r="E10">
+      <c r="G10" s="1">
         <f>0.25 + 0.6</f>
         <v>0.85</v>
       </c>
-      <c r="F10">
+      <c r="H10" s="1">
         <v>0.5</v>
       </c>
-      <c r="H10">
+      <c r="I10" s="2"/>
+      <c r="J10" s="5">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="N10">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="4">
         <f>0.07 + 0.008</f>
         <v>7.8000000000000014E-2</v>
       </c>
-      <c r="O10">
+      <c r="Q10" s="4">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="P10">
+      <c r="R10" s="5">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="Q10">
+      <c r="S10" s="5">
         <f>3*0.00035</f>
         <v>1.0499999999999999E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1.8</v>
       </c>
-      <c r="D11">
+      <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>0.58499999999999996</v>
       </c>
-      <c r="H11">
+      <c r="D11" s="1">
+        <f>E11</f>
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="E11" s="1">
+        <f>F11 * B11</f>
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="5">
         <v>0.01</v>
       </c>
-      <c r="I11">
+      <c r="K11" s="3">
         <v>0.16500000000000001</v>
       </c>
-      <c r="J11">
+      <c r="L11" s="3">
         <f>0.35 + 0.06</f>
         <v>0.41</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="M11" s="3"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>1.2</v>
       </c>
-      <c r="D12">
+      <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E12">
+      <c r="D12" s="1">
+        <f>E12</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="E12" s="1">
+        <f>F12 * B12</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>6</v>
       </c>
-      <c r="C13">
-        <f>D15 + D17</f>
-        <v>0.47099999999999997</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.64013333333333333</v>
+      </c>
+      <c r="D13" s="3">
+        <f>(B13 - B15)*D15 + (B13 - B17) *D17</f>
+        <v>3.8408000000000002</v>
+      </c>
+      <c r="E13" s="3">
+        <f>F13 * B13</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>-6</v>
       </c>
-      <c r="C14">
-        <f>D16</f>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>-7.5833333333333322E-2</v>
+      </c>
+      <c r="D14" s="3">
+        <f>(B14 - B16) * D16</f>
+        <v>0.45499999999999996</v>
+      </c>
+      <c r="E14" s="3">
+        <f>F14 * B14</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
+      <c r="D15" s="3">
+        <f>E15</f>
+        <v>0.45499999999999996</v>
+      </c>
+      <c r="E15" s="3">
+        <f>F15 * B15</f>
+        <v>0.45499999999999996</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="1"/>
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="K15">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3">
         <f>0.025 + 0.066</f>
         <v>9.0999999999999998E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>-5</v>
       </c>
-      <c r="D16">
+      <c r="C16" s="3">
         <f t="shared" si="0"/>
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="K16">
+      <c r="D16" s="3">
+        <f>E16</f>
+        <v>-0.45499999999999996</v>
+      </c>
+      <c r="E16" s="3">
+        <f>F16 * B16</f>
+        <v>-0.45499999999999996</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3">
         <f>0.025 + 0.066</f>
         <v>9.0999999999999998E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>3.3</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
+      <c r="C17" s="3">
+        <f>D17 / B17</f>
         <v>0.38</v>
       </c>
-      <c r="I17">
+      <c r="D17" s="3">
+        <f>E17</f>
+        <v>1.254</v>
+      </c>
+      <c r="E17" s="3">
+        <f>F17 * B17</f>
+        <v>1.254</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="1"/>
+        <v>0.38</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="3">
         <v>0.32</v>
       </c>
-      <c r="J17">
+      <c r="L17" s="3">
         <v>0.06</v>
       </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
getting on the DRC
</commit_message>
<xml_diff>
--- a/Power.xlsx
+++ b/Power.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\UdeS_S7_APP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2447F5B4-6C78-46B9-8896-7EB82D8467DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F0B8DC-1E7B-452E-88D8-0FB8900D0C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,9 +603,12 @@
       </c>
       <c r="C3" s="10">
         <f t="shared" ref="C3:C16" si="0">D3 / B3</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="10"/>
+        <v>1.7356325189393935</v>
+      </c>
+      <c r="D3" s="10">
+        <f>(B3-B4) * (D4  / B4)</f>
+        <v>41.655180454545444</v>
+      </c>
       <c r="E3" s="10">
         <f>F3 * B3</f>
         <v>0</v>
@@ -637,9 +640,12 @@
       </c>
       <c r="C4" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="10"/>
+        <v>3.471265037878787</v>
+      </c>
+      <c r="D4" s="10">
+        <f>(B4 - B7) * F7 + (B4 - B10) * (D10 / B10) + (B4 - B13) * (D13 / B13) + (B4 - B14) * (D14 / B14)</f>
+        <v>41.655180454545444</v>
+      </c>
       <c r="E4" s="10">
         <f>F4 * B4</f>
         <v>0</v>
@@ -671,9 +677,12 @@
       </c>
       <c r="C5" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="10"/>
+        <v>2.0300833333333332</v>
+      </c>
+      <c r="D5" s="10">
+        <f>E5 + (B5 - B6) * F6</f>
+        <v>48.722000000000001</v>
+      </c>
       <c r="E5" s="10">
         <f>F5 * B5</f>
         <v>48</v>
@@ -707,9 +716,12 @@
       </c>
       <c r="C6" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="10"/>
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D6" s="10">
+        <f>E6</f>
+        <v>0.19</v>
+      </c>
       <c r="E6" s="10">
         <f>F6 * B6</f>
         <v>0.19</v>
@@ -744,16 +756,19 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="2">
+        <f>(B7 - B8) * F8</f>
+        <v>0.75</v>
+      </c>
       <c r="E7" s="2">
         <f>F7 * B7</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>D7 / B7</f>
+        <v>0.3</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -778,9 +793,12 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="2">
+        <f>E8 + D9</f>
+        <v>1.125</v>
+      </c>
       <c r="E8" s="2">
         <f>F8 * B8</f>
         <v>1.125</v>
@@ -816,7 +834,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <f>E9</f>
+        <v>0</v>
+      </c>
       <c r="E9" s="2">
         <f>F9 * B9</f>
         <v>0</v>
@@ -985,11 +1006,11 @@
       </c>
       <c r="C13" s="3">
         <f t="shared" si="0"/>
-        <v>0.64013333333333333</v>
+        <v>0.18616666666666667</v>
       </c>
       <c r="D13" s="3">
-        <f>(B13 - B15)*D15 + (B13 - B17) *D17</f>
-        <v>3.8408000000000002</v>
+        <f>(B13 - B15)*F15 + (B13 - B17) * F17</f>
+        <v>1.117</v>
       </c>
       <c r="E13" s="3">
         <f>F13 * B13</f>
@@ -1022,11 +1043,11 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" si="0"/>
-        <v>-7.5833333333333322E-2</v>
+        <v>1.5166666666666667E-2</v>
       </c>
       <c r="D14" s="3">
-        <f>(B14 - B16) * D16</f>
-        <v>0.45499999999999996</v>
+        <f>(B14 - B16) * F16</f>
+        <v>-9.0999999999999998E-2</v>
       </c>
       <c r="E14" s="3">
         <f>F14 * B14</f>

</xml_diff>